<commit_message>
Added min_in_rot parameter for Green manure
</commit_message>
<xml_diff>
--- a/scenario_lab.xlsx
+++ b/scenario_lab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="DemandAndConversions" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="LayerHerd" sheetId="6" r:id="rId6"/>
     <sheet name="WasteAndCircularity" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="97">
   <si>
     <t>f_food</t>
   </si>
@@ -332,6 +332,21 @@
   </si>
   <si>
     <t>food waste, processing</t>
+  </si>
+  <si>
+    <t>Green manure</t>
+  </si>
+  <si>
+    <t>min_in_rot</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>This parameter controls the minimum share of cropland that must be</t>
+  </si>
+  <si>
+    <t>devoted to N-fixing green manures in each region</t>
   </si>
 </sst>
 </file>
@@ -429,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -462,6 +477,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -746,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,16 +1252,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1526,8 +1548,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="15">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jO/cnuACEkjTzqw4SaiWtg90AkKSjE1lV7AmdYfJ5UXV+CMS9MAlgfSSDNGdJ0mnZ2T4h5sQfX5dEgEsEd+Ltg==" saltValue="amFvgSCpMgdeJfKRW7QxRg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4K4JSKz8dhMjfuE4EjmvBfe1pz2mlXN2IqrmuhZ5rHsS1p7gMhWfaCLdJbjy6r0ZkoBdZuAWIMtbYFESbwJc/Q==" saltValue="uRHYyTntJGIH4IkHzYkwIg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1872,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -1971,7 +2023,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2122,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,7 +2204,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix beef/milk problem + improved scenario Excel workbook
</commit_message>
<xml_diff>
--- a/scenario_lab.xlsx
+++ b/scenario_lab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23880" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="DemandAndConversions" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="106">
   <si>
     <t>f_food</t>
   </si>
@@ -348,13 +348,41 @@
   <si>
     <t>devoted to N-fixing green manures in each region</t>
   </si>
+  <si>
+    <t>default values (avg.)</t>
+  </si>
+  <si>
+    <t>kg/ha</t>
+  </si>
+  <si>
+    <t>kg/m2</t>
+  </si>
+  <si>
+    <t>kg dm/ha</t>
+  </si>
+  <si>
+    <t>kg c.w.</t>
+  </si>
+  <si>
+    <t>kg/cow/year</t>
+  </si>
+  <si>
+    <t>kg/hen/year</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>kg feed/kg live weight gain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -444,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -485,6 +513,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,7 +813,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1309,7 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1296,35 +1340,28 @@
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="L1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="L2" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="11">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
@@ -1343,10 +1380,16 @@
       <c r="J3" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="18">
+        <v>6915.2247850000003</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>40</v>
@@ -1365,13 +1408,13 @@
       <c r="J4" s="12">
         <v>1</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="18">
+        <v>4641.2983690000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -1390,13 +1433,16 @@
       <c r="J5" s="12">
         <v>1</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="18">
+        <v>3338.21137</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
@@ -1415,10 +1461,16 @@
       <c r="J6" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="18">
+        <v>3301.9742179999998</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>40</v>
@@ -1437,10 +1489,13 @@
       <c r="J7" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="18">
+        <v>38501.085951000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>40</v>
@@ -1459,10 +1514,16 @@
       <c r="J8" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="18">
+        <v>4960.5618260000001</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>40</v>
@@ -1481,10 +1542,14 @@
       <c r="J9" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="18">
+        <v>30792.637392000001</v>
+      </c>
+      <c r="M9" s="21"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>40</v>
@@ -1503,10 +1568,14 @@
       <c r="J10" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="18">
+        <v>6024.6128529999996</v>
+      </c>
+      <c r="M10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>40</v>
@@ -1525,10 +1594,14 @@
       <c r="J11" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="18">
+        <v>16037.315522000001</v>
+      </c>
+      <c r="M11" s="21"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
@@ -1547,39 +1620,79 @@
       <c r="J12" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="L12" s="18">
+        <v>38.250456999999997</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="L13" s="19">
+        <v>3.1608179999999999</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D15" s="8">
         <v>0</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="15">
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="15">
         <v>0</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L15" s="10">
+        <v>0</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="N15" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L15" s="4" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="4" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4K4JSKz8dhMjfuE4EjmvBfe1pz2mlXN2IqrmuhZ5rHsS1p7gMhWfaCLdJbjy6r0ZkoBdZuAWIMtbYFESbwJc/Q==" saltValue="uRHYyTntJGIH4IkHzYkwIg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8GHcCfMN/MsA2uzQMllaN5P6RN1WI/27Lf2JetCQWHAXyTpcNxMMJNHL2qKPFVZmHXQD5tkoXK3rsV1Bcupfmg==" saltValue="ZenzDx5KG9qTGWOYcB1RqQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1587,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,7 +1713,7 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1631,8 +1744,11 @@
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>53</v>
       </c>
@@ -1643,8 +1759,9 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
@@ -1662,22 +1779,29 @@
       <c r="J3" s="9">
         <v>1</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="18">
+        <v>8819.5001499999998</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3" s="17"/>
+      <c r="O3" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" s="8"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="8"/>
-      <c r="L4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -1688,11 +1812,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
-      <c r="L5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>59</v>
       </c>
@@ -1713,11 +1837,18 @@
       <c r="J6" s="9">
         <v>1</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="22">
+        <v>305.63752899999997</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" s="17"/>
+      <c r="O6" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>62</v>
       </c>
@@ -1738,8 +1869,15 @@
       <c r="J7" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="22">
+        <v>330.03043400000001</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>63</v>
       </c>
@@ -1760,11 +1898,18 @@
       <c r="J8" s="9">
         <v>1</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="22">
+        <v>340.58024699999999</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" s="17"/>
+      <c r="O8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -1772,11 +1917,11 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="L9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -1785,7 +1930,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1794,7 +1939,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1832,11 +1977,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
@@ -1875,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>63</v>
       </c>
@@ -1915,17 +2060,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6jel3+2qZzu1P3BZX8Vt/Y2NWEUaG7nSP+yO0rOJEuVyaBbHpHAxP/UyBm4K+H3YuVGk5on+mouvLjkSyzY/+w==" saltValue="GzZKjx7hwUj/C52r7Qq+XA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bestvgzoQdwAZCbetzMm+CRAd95KLqEB2bLWAYA3c5L3Gni2QCTJVOJRydBJFTj67igoBpCTFOvABhCBdO/+gQ==" saltValue="R55syuI12qZjCKM5O2Xirg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,7 +2080,7 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1966,64 +2111,85 @@
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="L1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="L2" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>91.809441000000007</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L3" s="4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="4" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="4" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L7" s="4" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="4" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="k5F/okCg+aT0wRRGukgtwsWtP+gs0EotQNO8LcbM4wBsHSMk0bK3pdoE/wGb76DRtWsN9kdmDwEx6aQjOty52g==" saltValue="xAj4n/qeSew4F/RNzjH6AA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Z5pnxQojndoqDWwvsbqiVRJsFAAK4dJLsU7bnl29/zJynlNLRzUyyX38MyjEPy6Ok8q1dNFLIPaE7Fbt44ltxw==" saltValue="VTJ3riS8oAA3yGamuZCi6w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2200,7 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -2065,64 +2231,85 @@
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="L1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="L2" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1.52</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L3" s="4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="4" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="4" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L7" s="4" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="4" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7w698IJLxkSHylTqQ/BFMLq82xDb2+fljG7+yOEIEWdczIqgijNXmgH5mklDZnkTDv98aBLd9LDtoSLEis5vmQ==" saltValue="GSs8oo/GOwMxFQEKowa9wg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UoqNZhs+a5s/ku0JSqG11NIQaC2tjCa6cLSRdqOeitIFbcb57NcALxcQSGiThh5Eb1/DWcV2XeIzsFyHcGXJ1A==" saltValue="oSg+oJBycXBWS7wAD6jHRA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2319,7 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2160,41 +2347,61 @@
       <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="K1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="K3" s="8">
+        <v>18.047626000000001</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K4" s="4" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K5" s="4" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KcVDM91YLNdQ0Be1CqEPRJE2E3soZMOn2K5lcZRSA8aHRDhEYr7d1d0gnX9TYQWQvAU6iNo9hnsYptNRL1/qtg==" saltValue="jlSktQmvKKV3lg+swdxU2g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kxW3Ggw1h10rQcCI/bqvrOfONJDhsYZwHZeIXyEsbJoioIewwP8IZIa7DIWsP9bBouTUmJpEDiuUgHoF00xSyA==" saltValue="NgMzv8piWZpP9hZIoLGbGg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2204,7 +2411,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>